<commit_message>
limited and balanced attrition - analysis for internal validity
</commit_message>
<xml_diff>
--- a/Tables/SS_att.xlsx
+++ b/Tables/SS_att.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760AA09C-AB4E-40ED-92D1-9B31189F1C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C224A35-EA5B-428D-BD64-F77B7A98D779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18555" yWindow="-12060" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20415" yWindow="-13920" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_att" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Choice</t>
   </si>
@@ -495,7 +495,7 @@
   <dimension ref="B2:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,21 +514,21 @@
         <v>32.920245398773005</v>
       </c>
       <c r="L2">
-        <v>0.1902770180625333</v>
+        <v>0.2143179767360707</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>1.9667219667708402</v>
+        <v>5.542750930416787</v>
       </c>
       <c r="C3">
-        <v>2.0815298460890306</v>
+        <v>5.4215023872031063</v>
       </c>
       <c r="D3">
-        <v>1.9726264359542436</v>
+        <v>6.4065352622928202</v>
       </c>
       <c r="E3">
-        <v>1.1666513122535367</v>
+        <v>5.6071077586561913</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
@@ -562,21 +562,21 @@
         <v>23.153374233128833</v>
       </c>
       <c r="L5">
-        <v>0.1044644736090324</v>
+        <v>0.24002185859374711</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>1.1702249898250747</v>
+        <v>3.310190765365125</v>
       </c>
       <c r="C6">
-        <v>1.3872469067299058</v>
+        <v>3.7864915268436734</v>
       </c>
       <c r="D6">
-        <v>1.2628392959816359</v>
+        <v>4.3363271177356166</v>
       </c>
       <c r="E6">
-        <v>0.74273788684464404</v>
+        <v>3.7505032213798595</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -610,21 +610,21 @@
         <v>0.97049377759935773</v>
       </c>
       <c r="L10">
-        <v>0.61894128114173275</v>
+        <v>0.61894128114173319</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>5.5641049658199937E-3</v>
+        <v>5.5641049658199902E-3</v>
       </c>
       <c r="C11">
-        <v>9.0558404602785834E-3</v>
+        <v>9.0558404602785851E-3</v>
       </c>
       <c r="D11">
         <v>7.7705794497818937E-3</v>
       </c>
       <c r="E11">
-        <v>4.4762159277795628E-3</v>
+        <v>4.476215927779561E-3</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
@@ -655,7 +655,18 @@
         <v>2.4956672691430013E-2</v>
       </c>
       <c r="E13">
-        <v>1.3655060595903191E-2</v>
+        <v>1.365506059590319E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>1770</v>
+      </c>
+      <c r="C14">
+        <v>1954</v>
+      </c>
+      <c r="D14">
+        <v>2580</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
@@ -687,10 +698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754403B8-1DA5-4CBA-B8B6-94BFF0A849DB}">
-  <dimension ref="A3:S25"/>
+  <dimension ref="A3:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E16"/>
+      <selection activeCell="A4" sqref="A4:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -749,21 +760,21 @@
       </c>
       <c r="E6" s="1">
         <f>ROUND(SS_att!L2,2)</f>
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,1),")")</f>
-        <v>(2)</v>
+        <v>(5.5)</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C3,1),")")</f>
-        <v>(2.1)</v>
+        <v>(5.4)</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D3,1),")")</f>
-        <v>(2)</v>
+        <v>(6.4)</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -811,7 +822,7 @@
       </c>
       <c r="E9" s="6">
         <f>ROUND(SS_att!L5,2)</f>
-        <v>0.1</v>
+        <v>0.24</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -820,15 +831,15 @@
     <row r="10" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B6,1),")")</f>
-        <v>(1.2)</v>
+        <v>(3.3)</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C6,1),")")</f>
-        <v>(1.4)</v>
+        <v>(3.8)</v>
       </c>
       <c r="D10" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D6,1),")")</f>
-        <v>(1.3)</v>
+        <v>(4.3)</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -861,49 +872,50 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6">
-        <f>ROUND(SS_att!B10,2)</f>
-        <v>0.98</v>
-      </c>
-      <c r="C12" s="6">
-        <f>ROUND(SS_att!C10,2)</f>
-        <v>0.97</v>
-      </c>
-      <c r="D12" s="6">
-        <f>ROUND(SS_att!D10,2)</f>
-        <v>0.97</v>
-      </c>
-      <c r="E12" s="6">
-        <f>ROUND(SS_att!L10,2)</f>
-        <v>0.62</v>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+    <row r="12" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10">
+        <f>SS_att!B18</f>
+        <v>101</v>
+      </c>
+      <c r="C12" s="10">
+        <f>SS_att!C18</f>
+        <v>97</v>
+      </c>
+      <c r="D12" s="10">
+        <f>SS_att!D18</f>
+        <v>129</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B13" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!B11,2),")")</f>
-        <v>(0.01)</v>
-      </c>
-      <c r="C13" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!C11,2),")")</f>
-        <v>(0.01)</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!D11,2),")")</f>
-        <v>(0.01)</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+    <row r="13" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6">
+        <f>ROUND(SS_att!B10,2)</f>
+        <v>0.98</v>
+      </c>
+      <c r="C13" s="6">
+        <f>ROUND(SS_att!C10,2)</f>
+        <v>0.97</v>
+      </c>
+      <c r="D13" s="6">
+        <f>ROUND(SS_att!D10,2)</f>
+        <v>0.97</v>
+      </c>
+      <c r="E13" s="6">
+        <f>ROUND(SS_att!L10,2)</f>
+        <v>0.62</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -912,24 +924,17 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1">
-        <f>ROUND(SS_att!B12,2)</f>
-        <v>0.79</v>
-      </c>
-      <c r="C14" s="1">
-        <f>ROUND(SS_att!C12,2)</f>
-        <v>0.76</v>
-      </c>
-      <c r="D14" s="1">
-        <f>ROUND(SS_att!D12,2)</f>
-        <v>0.77</v>
-      </c>
-      <c r="E14" s="1">
-        <f>ROUND(SS_att!L12,2)</f>
-        <v>0.62</v>
+      <c r="B14" s="1" t="str">
+        <f>CONCATENATE("(",ROUND(SS_att!B11,2),")")</f>
+        <v>(0.01)</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>CONCATENATE("(",ROUND(SS_att!C11,2),")")</f>
+        <v>(0.01)</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>CONCATENATE("(",ROUND(SS_att!D11,2),")")</f>
+        <v>(0.01)</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -942,17 +947,24 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B15" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!B13,2),")")</f>
-        <v>(0.02)</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!C13,2),")")</f>
-        <v>(0.02)</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f>CONCATENATE("(",ROUND(SS_att!D13,2),")")</f>
-        <v>(0.02)</v>
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1">
+        <f>ROUND(SS_att!B12,2)</f>
+        <v>0.79</v>
+      </c>
+      <c r="C15" s="1">
+        <f>ROUND(SS_att!C12,2)</f>
+        <v>0.76</v>
+      </c>
+      <c r="D15" s="1">
+        <f>ROUND(SS_att!D12,2)</f>
+        <v>0.77</v>
+      </c>
+      <c r="E15" s="1">
+        <f>ROUND(SS_att!L12,2)</f>
+        <v>0.62</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -964,23 +976,19 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="10">
-        <f>SS_att!B18</f>
-        <v>101</v>
-      </c>
-      <c r="C16" s="10">
-        <f>SS_att!C18</f>
-        <v>97</v>
-      </c>
-      <c r="D16" s="10">
-        <f>SS_att!D18</f>
-        <v>129</v>
-      </c>
-      <c r="E16" s="10"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="str">
+        <f>CONCATENATE("(",ROUND(SS_att!B13,2),")")</f>
+        <v>(0.02)</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>CONCATENATE("(",ROUND(SS_att!C13,2),")")</f>
+        <v>(0.02)</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>CONCATENATE("(",ROUND(SS_att!D13,2),")")</f>
+        <v>(0.02)</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -991,7 +999,23 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="6:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="10">
+        <f>SS_att!B14</f>
+        <v>1770</v>
+      </c>
+      <c r="C17" s="10">
+        <f>SS_att!C14</f>
+        <v>1954</v>
+      </c>
+      <c r="D17" s="10">
+        <f>SS_att!D14</f>
+        <v>2580</v>
+      </c>
+      <c r="E17" s="10"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1002,7 +1026,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="6:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1013,7 +1037,7 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="6:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1024,18 +1048,18 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="6:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="6:19" x14ac:dyDescent="0.35">
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1043,23 +1067,34 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="6:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="6:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="25" spans="6:19" x14ac:dyDescent="0.35">
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
First set of edits after R&R
</commit_message>
<xml_diff>
--- a/Tables/SS_att.xlsx
+++ b/Tables/SS_att.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBCE4AF-3156-4E2E-B33A-0980507A3FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B29F4F-ABEA-400F-AADE-F3F183F273B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-9735" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attrition" sheetId="2" r:id="rId1"/>
@@ -34,15 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
-  <si>
-    <t>Commitment arms</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Control</t>
-  </si>
-  <si>
-    <t>Forced</t>
   </si>
   <si>
     <t>Choice</t>
@@ -74,6 +68,9 @@
   <si>
     <t>Amt borrowed/borrower</t>
   </si>
+  <si>
+    <t>Structure</t>
+  </si>
 </sst>
 </file>
 
@@ -94,7 +91,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9958800012207406E-2"/>
+        <fgColor theme="0" tint="-4.9836725974303414E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,9 +176,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,388 +510,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF41C6C-670C-46BE-BD39-7394AEFE19B1}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E21"/>
+      <selection activeCell="A2" sqref="A2:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C2" s="13" t="s">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1">
-        <f>ROUND(SS_att!B2,2)</f>
-        <v>0.97</v>
-      </c>
-      <c r="C4" s="1">
-        <f>ROUND(SS_att!C2,2)</f>
-        <v>0.96</v>
-      </c>
-      <c r="D4" s="1">
-        <f>ROUND(SS_att!D2,2)</f>
-        <v>0.97</v>
-      </c>
-      <c r="E4">
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <f>ROUND(SS_att!B2,3)</f>
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="C3" s="1">
+        <f>ROUND(SS_att!C2,3)</f>
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="D3" s="1">
+        <f>ROUND(SS_att!D2,3)</f>
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="E3">
         <f>ROUND(SS_att!L2,2)</f>
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2" t="str">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B3,2),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="C5" s="2" t="str">
+      <c r="C4" s="2" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C3,2),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="D5" s="2" t="str">
+      <c r="D4" s="2" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D3,2),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <f>ROUND(SS_att!B5,1)</f>
         <v>20.8</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C5" s="1">
         <f>ROUND(SS_att!C5,1)</f>
         <v>22.2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D5" s="1">
         <f>ROUND(SS_att!D5,1)</f>
         <v>25.4</v>
       </c>
-      <c r="E6">
+      <c r="E5">
         <f>ROUND(SS_att!L5,2)</f>
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="str">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B6,2),")")</f>
         <v>(3.29)</v>
       </c>
-      <c r="C7" s="1" t="str">
+      <c r="C6" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C6,2),")")</f>
         <v>(3.9)</v>
       </c>
-      <c r="D7" s="1" t="str">
+      <c r="D6" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D6,2),")")</f>
         <v>(4.89)</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11">
         <f>ROUND(SS_att!B7,1)</f>
         <v>19</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C7" s="11">
         <f>ROUND(SS_att!C7,1)</f>
         <v>20</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D7" s="11">
         <f>ROUND(SS_att!D7,1)</f>
         <v>21</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E7" s="12">
         <f>ROUND(SS_att!L7,2)</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
         <f>ROUND(SS_att!B8,1)</f>
         <v>1.4</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C8" s="1">
         <f>ROUND(SS_att!C8,1)</f>
         <v>1.4</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D8" s="1">
         <f>ROUND(SS_att!D8,1)</f>
         <v>1.4</v>
       </c>
-      <c r="E9">
+      <c r="E8">
         <f>ROUND(SS_att!L8,2)</f>
         <v>0.43</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="str">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B9,2),")")</f>
         <v>(0.08)</v>
       </c>
-      <c r="C10" s="1" t="str">
+      <c r="C9" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C9,2),")")</f>
         <v>(0.04)</v>
       </c>
-      <c r="D10" s="1" t="str">
+      <c r="D9" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D9,2),")")</f>
         <v>(0.05)</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="11">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="11">
         <f>ROUND(SS_att!B10,1)</f>
         <v>1.4</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C10" s="11">
         <f>ROUND(SS_att!C10,1)</f>
         <v>1.3</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D10" s="11">
         <f>ROUND(SS_att!D10,1)</f>
         <v>1.3</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E10" s="12">
         <f>ROUND(SS_att!L10,2)</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
         <f>ROUND(SS_att!B11,1)</f>
         <v>31</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C11" s="1">
         <f>ROUND(SS_att!C11,1)</f>
         <v>31.3</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D11" s="1">
         <f>ROUND(SS_att!D11,1)</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="E12">
+      <c r="E11">
         <f>ROUND(SS_att!L11,2)</f>
         <v>0.24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="1" t="str">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B12,1),")")</f>
         <v>(5.8)</v>
       </c>
-      <c r="C13" s="1" t="str">
+      <c r="C12" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C12,1),")")</f>
         <v>(5.6)</v>
       </c>
-      <c r="D13" s="1" t="str">
+      <c r="D12" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D12,1),")")</f>
         <v>(7.9)</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="11">
         <f>ROUND(SS_att!B13,1)</f>
         <v>27</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C13" s="11">
         <f>ROUND(SS_att!C13,1)</f>
         <v>28</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D13" s="11">
         <f>ROUND(SS_att!D13,1)</f>
         <v>30</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E13" s="12">
         <f>ROUND(SS_att!L13,2)</f>
         <v>0.46</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
         <f>ROUND(SS_att!B14,1)</f>
         <v>2266.8000000000002</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C14" s="1">
         <f>ROUND(SS_att!C14,1)</f>
         <v>2094</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D14" s="1">
         <f>ROUND(SS_att!D14,1)</f>
         <v>2115.1999999999998</v>
       </c>
-      <c r="E15">
+      <c r="E14">
         <f>ROUND(SS_att!L14,2)</f>
         <v>0.18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="1" t="str">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B15,1),")")</f>
         <v>(101.8)</v>
       </c>
-      <c r="C16" s="1" t="str">
+      <c r="C15" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C15,1),")")</f>
         <v>(83.7)</v>
       </c>
-      <c r="D16" s="1" t="str">
+      <c r="D15" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D15,1),")")</f>
         <v>(99.9)</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="11">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="11">
         <f>ROUND(SS_att!B16,1)</f>
         <v>2154.3000000000002</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C16" s="11">
         <f>ROUND(SS_att!C16,1)</f>
         <v>2041</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D16" s="11">
         <f>ROUND(SS_att!D16,1)</f>
         <v>2047.5</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E16" s="12">
         <f>ROUND(SS_att!L16,2)</f>
         <v>0.65</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1">
         <f>ROUND(SS_att!B17,0)</f>
         <v>47877</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C17" s="1">
         <f>ROUND(SS_att!C17,0)</f>
         <v>47813</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D17" s="1">
         <f>ROUND(SS_att!D17,0)</f>
         <v>54780</v>
       </c>
-      <c r="E18">
+      <c r="E17">
         <f>ROUND(SS_att!L17,2)</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="1" t="str">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!B18,0),")")</f>
         <v>(8005)</v>
       </c>
-      <c r="C19" s="1" t="str">
+      <c r="C18" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!C18,0),")")</f>
         <v>(9436)</v>
       </c>
-      <c r="D19" s="1" t="str">
+      <c r="D18" s="1" t="str">
         <f>CONCATENATE("(",ROUND(SS_att!D18,0),")")</f>
         <v>(12587)</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="11">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="11">
         <f>ROUND(SS_att!B19,1)</f>
         <v>37520</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C19" s="11">
         <f>ROUND(SS_att!C19,1)</f>
         <v>39420</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D19" s="11">
         <f>ROUND(SS_att!D19,1)</f>
         <v>40850</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E19" s="12">
         <f>ROUND(SS_att!L19,2)</f>
         <v>0.73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="9">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="9">
         <f>SS_att!B24</f>
         <v>85</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C20" s="9">
         <f>SS_att!C24</f>
         <v>81</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D20" s="9">
         <f>SS_att!D24</f>
         <v>94</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C2:E2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -906,56 +890,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>0.96889035242149624</v>
+        <v>0.96716697936210128</v>
       </c>
       <c r="C2">
-        <v>0.95522016728365866</v>
+        <v>0.95470085470085497</v>
       </c>
       <c r="D2">
-        <v>0.97156528952301191</v>
+        <v>0.96133682830930534</v>
       </c>
       <c r="E2">
-        <v>0.96554982383891297</v>
+        <v>0.96092503987240829</v>
       </c>
       <c r="L2">
-        <v>0.52902317841581303</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.82203658081697284</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>1.1015929528930456E-2</v>
+        <v>1.0616477679248965E-2</v>
       </c>
       <c r="C3">
-        <v>1.4757531191437263E-2</v>
+        <v>1.4476326826305447E-2</v>
       </c>
       <c r="D3">
-        <v>1.1584651503599948E-2</v>
+        <v>1.3703690061123075E-2</v>
       </c>
       <c r="E3">
-        <v>7.3802564247118611E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+        <v>9.5934103196447153E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>1</v>
+        <v>2635</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2535</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3494</v>
       </c>
       <c r="E4">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+        <v>8664</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>20.776470588235295</v>
       </c>
@@ -972,7 +958,7 @@
         <v>0.1691803885055099</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3.2888156639438466</v>
       </c>
@@ -986,7 +972,7 @@
         <v>3.9734365911287006</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>19</v>
       </c>
@@ -1003,7 +989,7 @@
         <v>0.50118311045391817</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1.4327417782374792</v>
       </c>
@@ -1020,7 +1006,7 @@
         <v>0.42853848079004753</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8.3862594173112967E-2</v>
       </c>
@@ -1034,7 +1020,7 @@
         <v>5.3418110498534621E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1.375</v>
       </c>
@@ -1051,7 +1037,7 @@
         <v>0.59646785336928199</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>30.988235294117647</v>
       </c>
@@ -1068,7 +1054,7 @@
         <v>0.23681502093860621</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>5.7678268283646368</v>
       </c>
@@ -1082,7 +1068,7 @@
         <v>6.2628499521065297</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>27</v>
       </c>
@@ -1099,7 +1085,7 @@
         <v>0.45502160387753737</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2266.804165652653</v>
       </c>
@@ -1116,7 +1102,7 @@
         <v>0.17906670526311749</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>101.7844366934046</v>
       </c>
@@ -1130,7 +1116,7 @@
         <v>82.567953252697222</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2154.3333333333335</v>
       </c>
@@ -1147,7 +1133,7 @@
         <v>0.64551965054073679</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>47877.058823529413</v>
       </c>
@@ -1164,7 +1150,7 @@
         <v>0.3963355120011216</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>8004.7525865977886</v>
       </c>
@@ -1178,7 +1164,7 @@
         <v>9824.2069237899068</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>37520</v>
       </c>
@@ -1195,7 +1181,7 @@
         <v>0.73046586285710446</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>20.776470588235295</v>
       </c>
@@ -1206,7 +1192,7 @@
         <v>25.361702127659573</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>85</v>
       </c>

</xml_diff>